<commit_message>
after adding java mail api
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -65,13 +65,76 @@
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>cus_Lif1DhRXWwRUpg</t>
-  </si>
-  <si>
-    <t>cus_Lif1EAxBptEmSw</t>
-  </si>
-  <si>
-    <t>cus_Lif1CTBNFigZ9q</t>
+    <t>cus_Lj1sjwM4YV9p2I</t>
+  </si>
+  <si>
+    <t>cus_Lj1sOAiI4mUdRr</t>
+  </si>
+  <si>
+    <t>cus_Lj1sYclhwbI5jQ</t>
+  </si>
+  <si>
+    <t>cus_Lj1ryzYh8gGfCX</t>
+  </si>
+  <si>
+    <t>cus_Lj1rmfOczqlhF5</t>
+  </si>
+  <si>
+    <t>cus_Lj1r5jc4SiZbY2</t>
+  </si>
+  <si>
+    <t>cus_LixxC5zDMvX4hp</t>
+  </si>
+  <si>
+    <t>cus_LixxSxX3HA3WQP</t>
+  </si>
+  <si>
+    <t>cus_LixxfBxSPabjHI</t>
+  </si>
+  <si>
+    <t>cus_LigOyXqqT5j9ls</t>
+  </si>
+  <si>
+    <t>cus_LigObgiOZVWTzZ</t>
+  </si>
+  <si>
+    <t>cus_LigOPUIj43ZELc</t>
+  </si>
+  <si>
+    <t>cus_LifMUzfnGKmBoz</t>
+  </si>
+  <si>
+    <t>cus_LifM6nLEZCLKq7</t>
+  </si>
+  <si>
+    <t>cus_LifMlrqjwRKPRZ</t>
+  </si>
+  <si>
+    <t>cus_LifESzNhWEB74Y</t>
+  </si>
+  <si>
+    <t>cus_LifENDKWOcz3qH</t>
+  </si>
+  <si>
+    <t>cus_LifERMKVrWRC9q</t>
+  </si>
+  <si>
+    <t>cus_Lif4IrNFXq3yyn</t>
+  </si>
+  <si>
+    <t>cus_Lif4jHeB4HZUpJ</t>
+  </si>
+  <si>
+    <t>cus_Lif4hz73M9gdtF</t>
+  </si>
+  <si>
+    <t>cus_LibCeM6Nmdmq40</t>
+  </si>
+  <si>
+    <t>cus_LibC7Yc31XkWZp</t>
+  </si>
+  <si>
+    <t>cus_LibC6ACVRYrJrP</t>
   </si>
 </sst>
 </file>
@@ -421,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,6 +594,111 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>